<commit_message>
Removed form class, refined dispersal method implementation
</commit_message>
<xml_diff>
--- a/docs/source/tutorials/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/docs/source/tutorials/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\docs\source\tutorials\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E502BE08-2572-410A-B882-616C3FB5D314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77086F9A-40E3-4933-8277-6327B6C34CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
     <sheet name="BTS" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DB!$A$1:$H$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DB!$A$1:$H$148</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="0">DB!$K$1:$K$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="241">
   <si>
     <t>Parameter</t>
   </si>
@@ -970,6 +970,9 @@
   </si>
   <si>
     <t>default uses relationships from Gao et al 2024 and Conti; min-max fits an long linear relationship between the minimum and maximum dimensions assuming proportionality with biomass or other dimensions by plant habit; for two-parameter relationships, the mean is used as well; user-defined requires the user to provide the best-fit relationship</t>
+  </si>
+  <si>
+    <t>translocation_rate</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1142,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1240,6 +1243,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1580,10 +1586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
-  <dimension ref="A1:K264"/>
+  <dimension ref="A1:K268"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1691,7 +1697,7 @@
         <v>178</v>
       </c>
       <c r="K4" t="str">
-        <f>E45</f>
+        <f>E49</f>
         <v>Poorter</v>
       </c>
     </row>
@@ -1716,7 +1722,7 @@
         <v>178</v>
       </c>
       <c r="K5" t="str">
-        <f>E60</f>
+        <f>E64</f>
         <v>Martinez-Vilalta</v>
       </c>
     </row>
@@ -1741,7 +1747,7 @@
         <v>178</v>
       </c>
       <c r="K6" t="str">
-        <f>E80</f>
+        <f>E84</f>
         <v>min-max</v>
       </c>
     </row>
@@ -1993,7 +1999,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="37" t="s">
         <v>224</v>
       </c>
       <c r="B19" s="19" t="s">
@@ -2019,7 +2025,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="36"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="19" t="s">
         <v>79</v>
       </c>
@@ -2040,7 +2046,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="36"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="19" t="s">
         <v>79</v>
       </c>
@@ -2061,7 +2067,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="36"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="19" t="s">
         <v>79</v>
       </c>
@@ -2267,7 +2273,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="38" t="s">
         <v>217</v>
       </c>
       <c r="B32" s="9" t="s">
@@ -2290,7 +2296,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="38"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="9" t="s">
         <v>75</v>
       </c>
@@ -2311,7 +2317,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="38"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="9" t="s">
         <v>75</v>
       </c>
@@ -2353,7 +2359,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="39" t="s">
         <v>219</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -2376,7 +2382,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="38"/>
+      <c r="A37" s="39"/>
       <c r="B37" s="9" t="s">
         <v>75</v>
       </c>
@@ -2397,7 +2403,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="38"/>
+      <c r="A38" s="39"/>
       <c r="B38" s="9" t="s">
         <v>75</v>
       </c>
@@ -2418,7 +2424,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="38"/>
+      <c r="A39" s="39"/>
       <c r="B39" s="9" t="s">
         <v>75</v>
       </c>
@@ -2438,101 +2444,82 @@
         <v>178</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="38" t="s">
-        <v>218</v>
-      </c>
+    <row r="40" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="36"/>
       <c r="B40" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>27</v>
+        <v>240</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>86</v>
       </c>
       <c r="E40" s="15">
-        <v>1.444</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="38"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="36"/>
       <c r="B41" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>27</v>
+        <v>240</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>87</v>
       </c>
       <c r="E41" s="15">
-        <v>1.5129999999999999</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="38"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="36"/>
       <c r="B42" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>27</v>
+        <v>240</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>88</v>
       </c>
       <c r="E42" s="15">
-        <v>1.4630000000000001</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="38"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="36"/>
       <c r="B43" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>27</v>
+        <v>240</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>78</v>
       </c>
       <c r="E43" s="15">
-        <v>1.4139999999999999</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="8"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="39" t="s">
+        <v>218</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" s="15">
+        <v>1.444</v>
+      </c>
       <c r="G44">
         <v>0</v>
       </c>
@@ -2540,22 +2527,19 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="39" t="s">
-        <v>28</v>
-      </c>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="39"/>
       <c r="B45" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="15">
+        <v>1.5129999999999999</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -2564,95 +2548,101 @@
         <v>178</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="40"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="39"/>
       <c r="B46" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="16"/>
+        <v>27</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" s="15">
+        <v>1.4630000000000001</v>
+      </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="40"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="39"/>
       <c r="B47" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E47" s="15"/>
+        <v>27</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" s="15">
+        <v>1.4139999999999999</v>
+      </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="40"/>
-      <c r="B48" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E48" s="15"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="8"/>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="40"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="40" t="s">
+        <v>28</v>
+      </c>
       <c r="B49" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E49" s="15"/>
+        <v>175</v>
+      </c>
+      <c r="D49" s="11"/>
+      <c r="E49" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="40"/>
+      <c r="A50" s="41"/>
       <c r="B50" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E50" s="15"/>
+      <c r="F50" s="16"/>
       <c r="G50">
         <v>0</v>
       </c>
@@ -2661,15 +2651,15 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="40"/>
+      <c r="A51" s="41"/>
       <c r="B51" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E51" s="15"/>
       <c r="G51">
@@ -2679,107 +2669,97 @@
         <v>192</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" s="36" t="s">
-        <v>33</v>
-      </c>
+    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="41"/>
       <c r="B52" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E52" s="15">
-        <v>0.01</v>
-      </c>
+      <c r="C52" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="15"/>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A53" s="36"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="41"/>
       <c r="B53" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E53" s="15">
-        <v>0.2</v>
-      </c>
+      <c r="C53" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" s="15"/>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" s="36"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="41"/>
       <c r="B54" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C54" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E54" s="15">
-        <v>0.5</v>
-      </c>
+      <c r="C54" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E54" s="15"/>
       <c r="G54">
         <v>0</v>
       </c>
       <c r="H54" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A55" s="25"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="41"/>
       <c r="B55" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E55" s="15">
-        <v>0</v>
-      </c>
+      <c r="C55" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="15"/>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A56" s="36" t="s">
-        <v>62</v>
+      <c r="A56" s="37" t="s">
+        <v>33</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>86</v>
       </c>
       <c r="E56" s="15">
-        <v>10.9</v>
+        <v>0.01</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2789,18 +2769,18 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A57" s="36"/>
+      <c r="A57" s="37"/>
       <c r="B57" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>87</v>
       </c>
       <c r="E57" s="15">
-        <v>6.68</v>
+        <v>0.2</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -2810,18 +2790,18 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A58" s="36"/>
+      <c r="A58" s="37"/>
       <c r="B58" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>88</v>
       </c>
       <c r="E58" s="15">
-        <v>10.02</v>
+        <v>0.5</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -2831,18 +2811,18 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A59" s="36"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>78</v>
       </c>
       <c r="E59" s="15">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2851,19 +2831,21 @@
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="30" t="s">
-        <v>179</v>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" s="37" t="s">
+        <v>62</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="15" t="s">
-        <v>177</v>
+        <v>63</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E60" s="15">
+        <v>10.9</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -2873,104 +2855,98 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A61" s="36" t="s">
-        <v>137</v>
-      </c>
+      <c r="A61" s="37"/>
       <c r="B61" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E61" s="15"/>
-      <c r="F61" s="16" t="s">
-        <v>136</v>
+        <v>63</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E61" s="15">
+        <v>6.68</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
       <c r="H61" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A62" s="36"/>
+      <c r="A62" s="37"/>
       <c r="B62" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D62" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E62" s="15"/>
-      <c r="F62" s="16" t="s">
-        <v>136</v>
+      <c r="E62" s="15">
+        <v>10.02</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A63" s="36"/>
+      <c r="A63" s="37"/>
       <c r="B63" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="E63" s="15"/>
-      <c r="F63" s="16" t="s">
-        <v>136</v>
+        <v>63</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E63" s="15">
+        <v>18</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
       <c r="H63" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A64" s="36"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A64" s="30" t="s">
+        <v>179</v>
+      </c>
       <c r="B64" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E64" s="15"/>
-      <c r="F64" s="16" t="s">
-        <v>136</v>
+        <v>176</v>
+      </c>
+      <c r="D64" s="18"/>
+      <c r="E64" s="15" t="s">
+        <v>177</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A65" s="36" t="s">
-        <v>138</v>
+      <c r="A65" s="37" t="s">
+        <v>137</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D65" s="17" t="s">
         <v>86</v>
@@ -2987,12 +2963,12 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A66" s="36"/>
+      <c r="A66" s="37"/>
       <c r="B66" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D66" s="17" t="s">
         <v>88</v>
@@ -3009,12 +2985,12 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A67" s="36"/>
+      <c r="A67" s="37"/>
       <c r="B67" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D67" s="17" t="s">
         <v>87</v>
@@ -3031,12 +3007,12 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" s="36"/>
+      <c r="A68" s="37"/>
       <c r="B68" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D68" s="17" t="s">
         <v>78</v>
@@ -3053,14 +3029,14 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A69" s="36" t="s">
-        <v>139</v>
+      <c r="A69" s="37" t="s">
+        <v>138</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D69" s="17" t="s">
         <v>86</v>
@@ -3077,12 +3053,12 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A70" s="36"/>
+      <c r="A70" s="37"/>
       <c r="B70" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D70" s="17" t="s">
         <v>88</v>
@@ -3099,12 +3075,12 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A71" s="36"/>
+      <c r="A71" s="37"/>
       <c r="B71" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D71" s="17" t="s">
         <v>87</v>
@@ -3121,12 +3097,12 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A72" s="36"/>
+      <c r="A72" s="37"/>
       <c r="B72" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D72" s="17" t="s">
         <v>78</v>
@@ -3143,14 +3119,14 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" s="36" t="s">
-        <v>140</v>
+      <c r="A73" s="37" t="s">
+        <v>139</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D73" s="17" t="s">
         <v>86</v>
@@ -3167,12 +3143,12 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" s="36"/>
+      <c r="A74" s="37"/>
       <c r="B74" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D74" s="17" t="s">
         <v>88</v>
@@ -3189,12 +3165,12 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A75" s="36"/>
+      <c r="A75" s="37"/>
       <c r="B75" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D75" s="17" t="s">
         <v>87</v>
@@ -3211,12 +3187,12 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A76" s="36"/>
+      <c r="A76" s="37"/>
       <c r="B76" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D76" s="17" t="s">
         <v>78</v>
@@ -3232,446 +3208,464 @@
         <v>193</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="5" t="s">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E77" s="15"/>
+      <c r="F77" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" s="37"/>
+      <c r="B78" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D78" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E78" s="15"/>
+      <c r="F78" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" s="37"/>
+      <c r="B79" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D79" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E79" s="15"/>
+      <c r="F79" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" s="37"/>
+      <c r="B80" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D80" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E80" s="15"/>
+      <c r="F80" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="8"/>
-      <c r="G77">
-        <v>0</v>
-      </c>
-      <c r="H77" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="19" t="s">
+      <c r="B81" s="5"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="8"/>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B78" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C78" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D78" s="18"/>
-      <c r="E78" s="15">
-        <v>100</v>
-      </c>
-      <c r="F78" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-      <c r="H78" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A79" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B79" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C79" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D79" s="18"/>
-      <c r="E79" s="15">
-        <v>9</v>
-      </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-      <c r="H79" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A80" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C80" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="D80" s="18"/>
-      <c r="E80" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="F80" t="s">
-        <v>239</v>
-      </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A81" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="D81" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="E81" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="H81" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A82" s="36"/>
       <c r="B82" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="D82" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="E82" s="15"/>
+        <v>36</v>
+      </c>
+      <c r="D82" s="18"/>
+      <c r="E82" s="15">
+        <v>100</v>
+      </c>
+      <c r="F82" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
       <c r="H82" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A83" s="36"/>
+      <c r="A83" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="B83" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="D83" s="18" t="s">
-        <v>230</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D83" s="18"/>
       <c r="E83" s="15">
-        <v>0.02</v>
+        <v>9</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
       </c>
       <c r="H83" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A84" s="36" t="s">
-        <v>232</v>
+      <c r="A84" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="B84" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="D84" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="E84" s="15">
-        <v>0.2</v>
+        <v>181</v>
+      </c>
+      <c r="D84" s="18"/>
+      <c r="E84" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="F84" t="s">
+        <v>239</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
       </c>
       <c r="H84" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A85" s="36"/>
+      <c r="A85" s="37" t="s">
+        <v>226</v>
+      </c>
       <c r="B85" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="E85" s="15"/>
+        <v>228</v>
+      </c>
+      <c r="E85" s="15">
+        <v>0.1</v>
+      </c>
       <c r="H85" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A86" s="36"/>
+      <c r="A86" s="37"/>
       <c r="B86" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="E86" s="15">
-        <v>0.06</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="E86" s="15"/>
       <c r="H86" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A87" s="36" t="s">
-        <v>233</v>
-      </c>
+      <c r="A87" s="37"/>
       <c r="B87" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C87" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="D87" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="E87" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="H87" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="B88" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="D88" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E88" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="H88" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89" s="37"/>
+      <c r="B89" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C89" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="D89" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E89" s="15"/>
+      <c r="H89" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90" s="37"/>
+      <c r="B90" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="D90" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="E90" s="15">
+        <v>0.06</v>
+      </c>
+      <c r="H90" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A91" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="B91" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C91" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="D87" s="18" t="s">
+      <c r="D91" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="E87" s="15">
+      <c r="E91" s="15">
         <f>0.91+3*0.007</f>
         <v>0.93100000000000005</v>
       </c>
-      <c r="H87" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A88" s="36"/>
-      <c r="B88" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="D88" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="E88" s="15"/>
-      <c r="H88" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A89" s="36"/>
-      <c r="B89" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C89" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="D89" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="E89" s="15">
-        <v>0.16</v>
-      </c>
-      <c r="H89" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A90" s="36" t="s">
-        <v>235</v>
-      </c>
-      <c r="B90" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C90" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="D90" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="E90" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="H90" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A91" s="36"/>
-      <c r="B91" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C91" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="D91" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="E91" s="15"/>
       <c r="H91" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A92" s="36"/>
+      <c r="A92" s="37"/>
       <c r="B92" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="E92" s="15">
-        <v>0.01</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="E92" s="15"/>
       <c r="H92" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A93" s="36" t="s">
-        <v>237</v>
-      </c>
+      <c r="A93" s="37"/>
       <c r="B93" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E93" s="15">
-        <v>1.45</v>
+        <v>0.16</v>
       </c>
       <c r="H93" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A94" s="36"/>
+      <c r="A94" s="37" t="s">
+        <v>235</v>
+      </c>
       <c r="B94" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="E94" s="15"/>
+        <v>228</v>
+      </c>
+      <c r="E94" s="15">
+        <v>0.5</v>
+      </c>
       <c r="H94" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A95" s="36"/>
+      <c r="A95" s="37"/>
       <c r="B95" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="E95" s="15">
-        <v>0.01</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="E95" s="15"/>
       <c r="H95" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A96" s="36" t="s">
-        <v>185</v>
-      </c>
+      <c r="A96" s="37"/>
       <c r="B96" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="D96" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E96" s="15"/>
-      <c r="G96">
-        <v>0</v>
+        <v>236</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="E96" s="15">
+        <v>0.01</v>
       </c>
       <c r="H96" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A97" s="36"/>
+      <c r="A97" s="37" t="s">
+        <v>237</v>
+      </c>
       <c r="B97" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="D97" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="E97" s="15"/>
-      <c r="G97">
-        <v>0</v>
+        <v>238</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E97" s="15">
+        <v>1.45</v>
       </c>
       <c r="H97" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A98" s="35"/>
+      <c r="A98" s="37"/>
       <c r="B98" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="D98" s="17" t="s">
-        <v>189</v>
+        <v>238</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>229</v>
       </c>
       <c r="E98" s="15"/>
+      <c r="H98" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A99" s="36" t="s">
-        <v>187</v>
-      </c>
+      <c r="A99" s="37"/>
       <c r="B99" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="D99" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E99" s="15"/>
-      <c r="G99">
-        <v>0</v>
+        <v>238</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="E99" s="15">
+        <v>0.01</v>
       </c>
       <c r="H99" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A100" s="36"/>
+      <c r="A100" s="37" t="s">
+        <v>185</v>
+      </c>
       <c r="B100" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="D100" s="17" t="s">
-        <v>186</v>
+        <v>29</v>
       </c>
       <c r="E100" s="15"/>
       <c r="G100">
@@ -3682,49 +3676,49 @@
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A101" s="35"/>
+      <c r="A101" s="37"/>
       <c r="B101" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="D101" s="17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E101" s="15"/>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A102" s="36" t="s">
-        <v>188</v>
-      </c>
+      <c r="A102" s="35"/>
       <c r="B102" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="D102" s="17" t="s">
-        <v>29</v>
+        <v>189</v>
       </c>
       <c r="E102" s="15"/>
-      <c r="G102">
-        <v>0</v>
-      </c>
-      <c r="H102" t="s">
-        <v>194</v>
-      </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A103" s="36"/>
+      <c r="A103" s="37" t="s">
+        <v>187</v>
+      </c>
       <c r="B103" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D103" s="17" t="s">
-        <v>186</v>
+        <v>29</v>
       </c>
       <c r="E103" s="15"/>
       <c r="G103">
@@ -3735,15 +3729,15 @@
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A104" s="36"/>
+      <c r="A104" s="37"/>
       <c r="B104" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D104" s="17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E104" s="15"/>
       <c r="G104">
@@ -3753,108 +3747,91 @@
         <v>194</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="19" t="s">
-        <v>144</v>
-      </c>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A105" s="35"/>
       <c r="B105" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D105" s="18"/>
-      <c r="E105" s="15">
-        <v>6.6309999999999997E-3</v>
-      </c>
-      <c r="G105">
-        <v>0</v>
-      </c>
-      <c r="H105" t="s">
-        <v>178</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="D105" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="E105" s="15"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A106" s="36" t="s">
-        <v>129</v>
+      <c r="A106" s="37" t="s">
+        <v>188</v>
       </c>
       <c r="B106" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C106" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="D106" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="E106" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F106" t="s">
-        <v>110</v>
-      </c>
+      <c r="C106" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D106" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E106" s="15"/>
       <c r="G106">
         <v>0</v>
       </c>
       <c r="H106" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A107" s="36"/>
+      <c r="A107" s="37"/>
       <c r="B107" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C107" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="D107" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="E107" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
+      <c r="C107" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D107" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="E107" s="15"/>
       <c r="G107">
         <v>0</v>
       </c>
       <c r="H107" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A108" s="36"/>
+      <c r="A108" s="37"/>
       <c r="B108" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C108" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="D108" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="E108" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
+      <c r="C108" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D108" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="E108" s="15"/>
       <c r="G108">
         <v>0</v>
       </c>
       <c r="H108" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A109" s="36"/>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A109" s="19" t="s">
+        <v>144</v>
+      </c>
       <c r="B109" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C109" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="D109" s="19" t="s">
-        <v>216</v>
-      </c>
+      <c r="C109" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D109" s="18"/>
       <c r="E109" s="15">
-        <v>7.0000000000000007E-2</v>
+        <v>6.6309999999999997E-3</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -3864,21 +3841,23 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A110" s="19" t="s">
-        <v>146</v>
+      <c r="A110" s="37" t="s">
+        <v>129</v>
       </c>
       <c r="B110" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D110" s="19"/>
+        <v>130</v>
+      </c>
+      <c r="D110" s="19" t="s">
+        <v>213</v>
+      </c>
       <c r="E110" s="15">
-        <v>3</v>
-      </c>
-      <c r="F110" s="19" t="s">
-        <v>148</v>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F110" t="s">
+        <v>110</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -3887,59 +3866,64 @@
         <v>178</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A111" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B111" s="5"/>
-      <c r="C111" s="6"/>
-      <c r="D111" s="7"/>
-      <c r="E111" s="6"/>
-      <c r="F111" s="8"/>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A111" s="37"/>
+      <c r="B111" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C111" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D111" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="E111" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="G111">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="H111" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="19" t="s">
-        <v>107</v>
-      </c>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A112" s="37"/>
       <c r="B112" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C112" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D112" s="18"/>
+        <v>76</v>
+      </c>
+      <c r="C112" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D112" s="19" t="s">
+        <v>215</v>
+      </c>
       <c r="E112" s="15">
-        <v>0.93600000000000005</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G112">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="H112" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A113" s="19" t="s">
-        <v>108</v>
-      </c>
+    <row r="113" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A113" s="37"/>
       <c r="B113" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C113" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D113" s="18"/>
+        <v>76</v>
+      </c>
+      <c r="C113" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D113" s="19" t="s">
+        <v>216</v>
+      </c>
       <c r="E113" s="15">
-        <v>0.5</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G113">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="H113" t="s">
         <v>178</v>
@@ -3947,21 +3931,23 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="19" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C114" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D114" s="18"/>
+        <v>76</v>
+      </c>
+      <c r="C114" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D114" s="19"/>
       <c r="E114" s="15">
-        <f>20*0.2*0.69</f>
-        <v>2.76</v>
+        <v>3</v>
+      </c>
+      <c r="F114" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="G114">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="H114" t="s">
         <v>178</v>
@@ -3969,15 +3955,15 @@
     </row>
     <row r="115" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A115" s="5" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="B115" s="5"/>
       <c r="C115" s="6"/>
       <c r="D115" s="7"/>
       <c r="E115" s="6"/>
-      <c r="F115" s="6"/>
+      <c r="F115" s="8"/>
       <c r="G115">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H115" t="s">
         <v>178</v>
@@ -3985,227 +3971,223 @@
     </row>
     <row r="116" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A116" s="19" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D116" s="18"/>
       <c r="E116" s="15">
-        <v>0.01</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="G116">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H116" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="19" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C117" s="17" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D117" s="18"/>
       <c r="E117" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G117">
+        <v>56</v>
+      </c>
+      <c r="H117" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A118" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B118" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D118" s="18"/>
+      <c r="E118" s="15">
+        <f>20*0.2*0.69</f>
+        <v>2.76</v>
+      </c>
+      <c r="G118">
+        <v>57</v>
+      </c>
+      <c r="H118" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A119" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B119" s="5"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="7"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119">
+        <v>58</v>
+      </c>
+      <c r="H119" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B120" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C120" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D120" s="18"/>
+      <c r="E120" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="G120">
+        <v>59</v>
+      </c>
+      <c r="H120" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A121" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B121" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C121" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D121" s="18"/>
+      <c r="E121" s="15">
         <v>365</v>
       </c>
-      <c r="H117" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A118" s="5" t="s">
+      <c r="H121" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A122" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B118" s="5"/>
-      <c r="C118" s="6"/>
-      <c r="D118" s="7"/>
-      <c r="E118" s="6"/>
-      <c r="F118" s="8" t="s">
+      <c r="B122" s="5"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="7"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G118">
+      <c r="G122">
         <v>60</v>
       </c>
-      <c r="H118" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="19" t="s">
+      <c r="H122" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B119" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C119" s="17" t="s">
+      <c r="B123" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C123" s="17" t="s">
         <v>72</v>
-      </c>
-      <c r="D119" s="18">
-        <v>1</v>
-      </c>
-      <c r="E119" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F119" t="s">
-        <v>89</v>
-      </c>
-      <c r="G119">
-        <v>61</v>
-      </c>
-      <c r="H119" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A120" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B120" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C120" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D120" s="18">
-        <v>1</v>
-      </c>
-      <c r="E120" s="15">
-        <v>207</v>
-      </c>
-      <c r="F120" t="s">
-        <v>94</v>
-      </c>
-      <c r="G120">
-        <v>62</v>
-      </c>
-      <c r="H120" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A121" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B121" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C121" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D121" s="18">
-        <v>1</v>
-      </c>
-      <c r="E121" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F121" t="s">
-        <v>95</v>
-      </c>
-      <c r="G121">
-        <v>63</v>
-      </c>
-      <c r="H121" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A122" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B122" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C122" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D122" s="18">
-        <v>1</v>
-      </c>
-      <c r="E122">
-        <v>20</v>
-      </c>
-      <c r="G122">
-        <v>64</v>
-      </c>
-      <c r="H122" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A123" s="19"/>
-      <c r="B123" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C123" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="D123" s="18">
         <v>1</v>
       </c>
-      <c r="E123" s="15">
-        <v>30</v>
+      <c r="E123" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F123" t="s">
+        <v>89</v>
       </c>
       <c r="G123">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H123" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A124" s="19"/>
+      <c r="A124" s="19" t="s">
+        <v>48</v>
+      </c>
       <c r="B124" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C124" s="17" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D124" s="18">
         <v>1</v>
       </c>
       <c r="E124" s="15">
-        <v>70</v>
+        <v>207</v>
+      </c>
+      <c r="F124" t="s">
+        <v>94</v>
       </c>
       <c r="G124">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H124" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A125" s="19"/>
+      <c r="A125" s="19" t="s">
+        <v>90</v>
+      </c>
       <c r="B125" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C125" s="17" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D125" s="18">
         <v>1</v>
       </c>
-      <c r="E125" s="15">
-        <v>100</v>
+      <c r="E125" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F125" t="s">
+        <v>95</v>
       </c>
       <c r="G125">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H125" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A126" s="19"/>
+      <c r="A126" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="B126" s="19" t="s">
         <v>82</v>
       </c>
@@ -4215,78 +4197,74 @@
       <c r="D126" s="18">
         <v>1</v>
       </c>
-      <c r="E126" s="15"/>
+      <c r="E126">
+        <v>20</v>
+      </c>
       <c r="G126">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H126" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A127" s="19" t="s">
-        <v>96</v>
-      </c>
+      <c r="A127" s="19"/>
       <c r="B127" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C127" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D127" s="18">
         <v>1</v>
       </c>
       <c r="E127" s="15">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G127">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H127" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A128" s="19" t="s">
-        <v>97</v>
-      </c>
+      <c r="A128" s="19"/>
       <c r="B128" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C128" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D128" s="18">
         <v>1</v>
       </c>
       <c r="E128" s="15">
-        <v>0.01</v>
+        <v>70</v>
       </c>
       <c r="G128">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H128" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A129" s="19" t="s">
-        <v>98</v>
-      </c>
+      <c r="A129" s="19"/>
       <c r="B129" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C129" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D129" s="18">
         <v>1</v>
       </c>
       <c r="E129" s="15">
-        <v>0.67</v>
+        <v>100</v>
       </c>
       <c r="G129">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H129" t="s">
         <v>178</v>
@@ -4298,20 +4276,23 @@
         <v>82</v>
       </c>
       <c r="C130" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D130" s="18">
         <v>1</v>
       </c>
-      <c r="E130" s="15">
-        <v>1</v>
+      <c r="E130" s="15"/>
+      <c r="G130">
+        <v>68</v>
       </c>
       <c r="H130" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A131" s="19"/>
+      <c r="A131" s="19" t="s">
+        <v>96</v>
+      </c>
       <c r="B131" s="19" t="s">
         <v>82</v>
       </c>
@@ -4321,9 +4302,11 @@
       <c r="D131" s="18">
         <v>1</v>
       </c>
-      <c r="E131" s="15"/>
+      <c r="E131" s="15">
+        <v>0</v>
+      </c>
       <c r="G131">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H131" t="s">
         <v>178</v>
@@ -4331,22 +4314,22 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="19" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="B132" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C132" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D132" s="18">
-        <v>2</v>
-      </c>
-      <c r="E132" s="12" t="s">
-        <v>128</v>
+        <v>1</v>
+      </c>
+      <c r="E132" s="15">
+        <v>0.01</v>
       </c>
       <c r="G132">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H132" t="s">
         <v>178</v>
@@ -4354,138 +4337,137 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="19" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B133" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C133" s="17" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D133" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E133" s="15">
-        <v>365</v>
+        <v>0.67</v>
       </c>
       <c r="G133">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H133" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A134" s="19" t="s">
-        <v>93</v>
-      </c>
+      <c r="A134" s="19"/>
       <c r="B134" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C134" s="17" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D134" s="18">
-        <v>2</v>
-      </c>
-      <c r="E134" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G134">
-        <v>80</v>
+        <v>1</v>
+      </c>
+      <c r="E134" s="15">
+        <v>1</v>
       </c>
       <c r="H134" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A135" s="19" t="s">
-        <v>53</v>
-      </c>
+      <c r="A135" s="19"/>
       <c r="B135" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C135" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D135" s="18">
-        <v>2</v>
-      </c>
-      <c r="E135" s="15">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E135" s="15"/>
       <c r="G135">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H135" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A136" s="19"/>
+      <c r="A136" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="B136" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C136" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D136" s="18">
         <v>2</v>
       </c>
-      <c r="E136" s="15">
-        <v>0.2</v>
+      <c r="E136" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="G136">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H136" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A137" s="19"/>
+      <c r="A137" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="B137" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C137" s="17" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D137" s="18">
         <v>2</v>
       </c>
       <c r="E137" s="15">
-        <v>0.5</v>
+        <v>365</v>
       </c>
       <c r="G137">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H137" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A138" s="19"/>
+      <c r="A138" s="19" t="s">
+        <v>93</v>
+      </c>
       <c r="B138" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C138" s="17" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D138" s="18">
         <v>2</v>
       </c>
-      <c r="E138" s="15">
-        <v>1.1200000000000001</v>
+      <c r="E138" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="G138">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H138" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A139" s="19"/>
+      <c r="A139" s="19" t="s">
+        <v>53</v>
+      </c>
       <c r="B139" s="19" t="s">
         <v>82</v>
       </c>
@@ -4496,73 +4478,73 @@
         <v>2</v>
       </c>
       <c r="E139" s="15">
-        <v>1.69</v>
+        <v>0</v>
       </c>
       <c r="G139">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H139" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A140" s="19" t="s">
-        <v>54</v>
-      </c>
+      <c r="A140" s="19"/>
       <c r="B140" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C140" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D140" s="18">
         <v>2</v>
       </c>
       <c r="E140" s="15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G140">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H140" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A141" s="19" t="s">
-        <v>97</v>
-      </c>
+      <c r="A141" s="19"/>
       <c r="B141" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C141" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D141" s="18">
         <v>2</v>
       </c>
       <c r="E141" s="15">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="G141">
+        <v>83</v>
       </c>
       <c r="H141" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A142" s="19" t="s">
-        <v>98</v>
-      </c>
+      <c r="A142" s="19"/>
       <c r="B142" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C142" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D142" s="18">
         <v>2</v>
       </c>
       <c r="E142" s="15">
-        <v>0.02</v>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G142">
+        <v>84</v>
       </c>
       <c r="H142" t="s">
         <v>178</v>
@@ -4574,20 +4556,25 @@
         <v>82</v>
       </c>
       <c r="C143" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D143" s="18">
         <v>2</v>
       </c>
       <c r="E143" s="15">
-        <v>1</v>
+        <v>1.69</v>
+      </c>
+      <c r="G143">
+        <v>85</v>
       </c>
       <c r="H143" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A144" s="19"/>
+      <c r="A144" s="19" t="s">
+        <v>54</v>
+      </c>
       <c r="B144" s="19" t="s">
         <v>82</v>
       </c>
@@ -4598,7 +4585,10 @@
         <v>2</v>
       </c>
       <c r="E144" s="15">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <v>86</v>
       </c>
       <c r="H144" t="s">
         <v>178</v>
@@ -4606,16 +4596,19 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" s="19" t="s">
-        <v>197</v>
+        <v>97</v>
       </c>
       <c r="B145" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C145" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D145" s="18">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E145" s="15">
+        <v>0</v>
       </c>
       <c r="H145" t="s">
         <v>178</v>
@@ -4623,62 +4616,69 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" s="19" t="s">
-        <v>199</v>
+        <v>98</v>
       </c>
       <c r="B146" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C146" s="17" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D146" s="18">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E146" s="15">
+        <v>0.02</v>
       </c>
       <c r="H146" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A147" s="19" t="s">
-        <v>200</v>
-      </c>
+      <c r="A147" s="19"/>
       <c r="B147" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C147" s="17" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D147" s="18">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E147" s="15">
+        <v>1</v>
       </c>
       <c r="H147" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A148" s="19" t="s">
-        <v>198</v>
-      </c>
+      <c r="A148" s="19"/>
       <c r="B148" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C148" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D148" s="18">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E148" s="15">
+        <v>1</v>
       </c>
       <c r="H148" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A149" s="19"/>
+      <c r="A149" s="19" t="s">
+        <v>197</v>
+      </c>
       <c r="B149" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C149" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D149" s="18">
         <v>3</v>
@@ -4688,12 +4688,14 @@
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A150" s="19"/>
+      <c r="A150" s="19" t="s">
+        <v>199</v>
+      </c>
       <c r="B150" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C150" s="17" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D150" s="18">
         <v>3</v>
@@ -4703,12 +4705,14 @@
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A151" s="19"/>
+      <c r="A151" s="19" t="s">
+        <v>200</v>
+      </c>
       <c r="B151" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C151" s="17" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D151" s="18">
         <v>3</v>
@@ -4718,7 +4722,9 @@
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A152" s="19"/>
+      <c r="A152" s="19" t="s">
+        <v>198</v>
+      </c>
       <c r="B152" s="19" t="s">
         <v>82</v>
       </c>
@@ -4733,14 +4739,12 @@
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A153" s="19" t="s">
-        <v>201</v>
-      </c>
+      <c r="A153" s="19"/>
       <c r="B153" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C153" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D153" s="18">
         <v>3</v>
@@ -4750,14 +4754,12 @@
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A154" s="19" t="s">
-        <v>97</v>
-      </c>
+      <c r="A154" s="19"/>
       <c r="B154" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C154" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D154" s="18">
         <v>3</v>
@@ -4767,14 +4769,12 @@
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A155" s="19" t="s">
-        <v>98</v>
-      </c>
+      <c r="A155" s="19"/>
       <c r="B155" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C155" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D155" s="18">
         <v>3</v>
@@ -4789,7 +4789,7 @@
         <v>82</v>
       </c>
       <c r="C156" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D156" s="18">
         <v>3</v>
@@ -4799,7 +4799,9 @@
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A157" s="19"/>
+      <c r="A157" s="19" t="s">
+        <v>201</v>
+      </c>
       <c r="B157" s="19" t="s">
         <v>82</v>
       </c>
@@ -4815,16 +4817,16 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" s="19" t="s">
-        <v>202</v>
+        <v>97</v>
       </c>
       <c r="B158" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C158" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D158" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H158" t="s">
         <v>178</v>
@@ -4832,62 +4834,60 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" s="19" t="s">
-        <v>204</v>
+        <v>98</v>
       </c>
       <c r="B159" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C159" s="17" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D159" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H159" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A160" s="19" t="s">
-        <v>205</v>
-      </c>
+      <c r="A160" s="19"/>
       <c r="B160" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C160" s="17" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D160" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H160" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A161" s="19" t="s">
-        <v>203</v>
-      </c>
+      <c r="A161" s="19"/>
       <c r="B161" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C161" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D161" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H161" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A162" s="19"/>
+      <c r="A162" s="19" t="s">
+        <v>202</v>
+      </c>
       <c r="B162" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C162" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D162" s="18">
         <v>4</v>
@@ -4897,12 +4897,14 @@
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A163" s="19"/>
+      <c r="A163" s="19" t="s">
+        <v>204</v>
+      </c>
       <c r="B163" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C163" s="17" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D163" s="18">
         <v>4</v>
@@ -4912,12 +4914,14 @@
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A164" s="19"/>
+      <c r="A164" s="19" t="s">
+        <v>205</v>
+      </c>
       <c r="B164" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C164" s="17" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D164" s="18">
         <v>4</v>
@@ -4927,7 +4931,9 @@
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A165" s="19"/>
+      <c r="A165" s="19" t="s">
+        <v>203</v>
+      </c>
       <c r="B165" s="19" t="s">
         <v>82</v>
       </c>
@@ -4942,14 +4948,12 @@
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A166" s="19" t="s">
-        <v>206</v>
-      </c>
+      <c r="A166" s="19"/>
       <c r="B166" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C166" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D166" s="18">
         <v>4</v>
@@ -4959,14 +4963,12 @@
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A167" s="19" t="s">
-        <v>97</v>
-      </c>
+      <c r="A167" s="19"/>
       <c r="B167" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C167" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D167" s="18">
         <v>4</v>
@@ -4976,14 +4978,12 @@
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A168" s="19" t="s">
-        <v>98</v>
-      </c>
+      <c r="A168" s="19"/>
       <c r="B168" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C168" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D168" s="18">
         <v>4</v>
@@ -4998,7 +4998,7 @@
         <v>82</v>
       </c>
       <c r="C169" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D169" s="18">
         <v>4</v>
@@ -5008,7 +5008,9 @@
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A170" s="19"/>
+      <c r="A170" s="19" t="s">
+        <v>206</v>
+      </c>
       <c r="B170" s="19" t="s">
         <v>82</v>
       </c>
@@ -5024,16 +5026,16 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="19" t="s">
-        <v>208</v>
+        <v>97</v>
       </c>
       <c r="B171" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C171" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D171" s="18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H171" t="s">
         <v>178</v>
@@ -5041,62 +5043,60 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" s="19" t="s">
-        <v>207</v>
+        <v>98</v>
       </c>
       <c r="B172" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C172" s="17" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D172" s="18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H172" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A173" s="19" t="s">
-        <v>209</v>
-      </c>
+      <c r="A173" s="19"/>
       <c r="B173" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C173" s="17" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D173" s="18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H173" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A174" s="19" t="s">
-        <v>210</v>
-      </c>
+      <c r="A174" s="19"/>
       <c r="B174" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C174" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D174" s="18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H174" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A175" s="19"/>
+      <c r="A175" s="19" t="s">
+        <v>208</v>
+      </c>
       <c r="B175" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C175" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D175" s="18">
         <v>5</v>
@@ -5106,12 +5106,14 @@
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A176" s="19"/>
+      <c r="A176" s="19" t="s">
+        <v>207</v>
+      </c>
       <c r="B176" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C176" s="17" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D176" s="18">
         <v>5</v>
@@ -5121,12 +5123,14 @@
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A177" s="19"/>
+      <c r="A177" s="19" t="s">
+        <v>209</v>
+      </c>
       <c r="B177" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C177" s="17" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D177" s="18">
         <v>5</v>
@@ -5136,7 +5140,9 @@
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A178" s="19"/>
+      <c r="A178" s="19" t="s">
+        <v>210</v>
+      </c>
       <c r="B178" s="19" t="s">
         <v>82</v>
       </c>
@@ -5151,14 +5157,12 @@
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A179" s="19" t="s">
-        <v>211</v>
-      </c>
+      <c r="A179" s="19"/>
       <c r="B179" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C179" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D179" s="18">
         <v>5</v>
@@ -5168,14 +5172,12 @@
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A180" s="19" t="s">
-        <v>97</v>
-      </c>
+      <c r="A180" s="19"/>
       <c r="B180" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C180" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D180" s="18">
         <v>5</v>
@@ -5185,14 +5187,12 @@
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A181" s="19" t="s">
-        <v>98</v>
-      </c>
+      <c r="A181" s="19"/>
       <c r="B181" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C181" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D181" s="18">
         <v>5</v>
@@ -5207,7 +5207,7 @@
         <v>82</v>
       </c>
       <c r="C182" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D182" s="18">
         <v>5</v>
@@ -5217,7 +5217,9 @@
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A183" s="19"/>
+      <c r="A183" s="19" t="s">
+        <v>211</v>
+      </c>
       <c r="B183" s="19" t="s">
         <v>82</v>
       </c>
@@ -5232,28 +5234,68 @@
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A184" s="20"/>
-      <c r="B184" s="20"/>
-      <c r="C184" s="21"/>
-      <c r="D184" s="22"/>
+      <c r="A184" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B184" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C184" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D184" s="18">
+        <v>5</v>
+      </c>
+      <c r="H184" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A185" s="20"/>
-      <c r="B185" s="20"/>
-      <c r="C185" s="21"/>
-      <c r="D185" s="22"/>
+      <c r="A185" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B185" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C185" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D185" s="18">
+        <v>5</v>
+      </c>
+      <c r="H185" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A186" s="20"/>
-      <c r="B186" s="20"/>
-      <c r="C186" s="21"/>
-      <c r="D186" s="22"/>
+      <c r="A186" s="19"/>
+      <c r="B186" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C186" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D186" s="18">
+        <v>5</v>
+      </c>
+      <c r="H186" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A187" s="20"/>
-      <c r="B187" s="20"/>
-      <c r="C187" s="21"/>
-      <c r="D187" s="22"/>
+      <c r="A187" s="19"/>
+      <c r="B187" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C187" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D187" s="18">
+        <v>5</v>
+      </c>
+      <c r="H187" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" s="20"/>
@@ -5659,21 +5701,25 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A255" s="20"/>
+      <c r="B255" s="20"/>
       <c r="C255" s="21"/>
       <c r="D255" s="22"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A256" s="20"/>
+      <c r="B256" s="20"/>
       <c r="C256" s="21"/>
       <c r="D256" s="22"/>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A257" s="20"/>
+      <c r="B257" s="20"/>
       <c r="C257" s="21"/>
       <c r="D257" s="22"/>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A258" s="20"/>
+      <c r="B258" s="20"/>
       <c r="C258" s="21"/>
       <c r="D258" s="22"/>
     </row>
@@ -5707,28 +5753,48 @@
       <c r="C264" s="21"/>
       <c r="D264" s="22"/>
     </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A265" s="20"/>
+      <c r="C265" s="21"/>
+      <c r="D265" s="22"/>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A266" s="20"/>
+      <c r="C266" s="21"/>
+      <c r="D266" s="22"/>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A267" s="20"/>
+      <c r="C267" s="21"/>
+      <c r="D267" s="22"/>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A268" s="20"/>
+      <c r="C268" s="21"/>
+      <c r="D268" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="A106:A108"/>
+    <mergeCell ref="A110:A113"/>
+    <mergeCell ref="A77:A80"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A91:A93"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="A97:A99"/>
     <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A61:A64"/>
     <mergeCell ref="A65:A68"/>
     <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A73:A76"/>
     <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A45:A51"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A49:A55"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A56:A58"/>
     <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="A106:A109"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="A87:A89"/>
-    <mergeCell ref="A90:A92"/>
-    <mergeCell ref="A93:A95"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="21">
@@ -5741,10 +5807,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{FCAB33B4-E22D-416A-9EE8-1B6629F4B7A9}">
       <formula1>"angiosperm, gymnosperm"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E117" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E121" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E118 E113 E115:E116 F115" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E122 E117 E119:E120 F119" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -5755,7 +5821,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10" xr:uid="{5620C1FF-B28B-4556-ADEF-5FA98FE67CB9}">
       <formula1>"C3, C4, CAM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E44 E23 E31" xr:uid="{D43B937F-2CE8-47D9-A978-7D336015DF11}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E48 E23 E31" xr:uid="{D43B937F-2CE8-47D9-A978-7D336015DF11}">
       <formula1>"Annual, Herbaceous perennial, Woody perennial"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10" xr:uid="{6E5E4A37-6A5B-480B-8E8F-63973FC4A36F}">
@@ -5767,7 +5833,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{793E17DF-C558-4DAF-B608-9E20297CD619}">
       <formula1>"annual, perennial evergreen, perennial deciduous"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E121 E134" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E125 E138" xr:uid="{C614F1BE-BCDD-4E7E-8FB4-A3D677A1BB44}">
       <formula1>"year-round, during growing season, during dormant season"</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E24" xr:uid="{DC451139-D175-47A3-922A-D7E1D89FD320}">
@@ -5790,13 +5856,13 @@
       <formula1>0</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E45" xr:uid="{E2339C9A-2940-4141-B685-7BF33B5A8E51}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E49" xr:uid="{E2339C9A-2940-4141-B685-7BF33B5A8E51}">
       <formula1>"Poorter, user-defined allocation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E60" xr:uid="{D19B13DA-06D3-4C4D-9900-E7890DE8817B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E64" xr:uid="{D19B13DA-06D3-4C4D-9900-E7890DE8817B}">
       <formula1>"Martinez-Vilalta, user-defined NSC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E80" xr:uid="{77DF1237-7A63-492D-A14F-5AB9AC22765E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E84" xr:uid="{77DF1237-7A63-492D-A14F-5AB9AC22765E}">
       <formula1>"min-max, user-defined allometry, default"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9" xr:uid="{3D116903-B405-4900-ADF4-C113E5F8EB27}">
@@ -6404,7 +6470,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="41" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="9" t="s">
@@ -6427,7 +6493,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="40"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="9" t="s">
         <v>75</v>
       </c>
@@ -6448,7 +6514,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="40"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="9" t="s">
         <v>75</v>
       </c>
@@ -6469,7 +6535,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="40"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="9" t="s">
         <v>75</v>
       </c>
@@ -6490,7 +6556,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="39" t="s">
         <v>219</v>
       </c>
       <c r="B32" s="9" t="s">
@@ -6513,7 +6579,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="38"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="9" t="s">
         <v>75</v>
       </c>
@@ -6534,7 +6600,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="38"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="9" t="s">
         <v>75</v>
       </c>
@@ -6555,7 +6621,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="38"/>
+      <c r="A35" s="39"/>
       <c r="B35" s="9" t="s">
         <v>75</v>
       </c>
@@ -6576,7 +6642,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="41" t="s">
         <v>26</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -6599,7 +6665,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="40"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="9" t="s">
         <v>75</v>
       </c>
@@ -6620,7 +6686,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="40"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="9" t="s">
         <v>75</v>
       </c>
@@ -6641,7 +6707,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="40"/>
+      <c r="A39" s="41"/>
       <c r="B39" s="9" t="s">
         <v>75</v>
       </c>
@@ -6700,7 +6766,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="42" t="s">
+      <c r="A42" s="43" t="s">
         <v>28</v>
       </c>
       <c r="B42" s="9" t="s">
@@ -6713,7 +6779,7 @@
         <v>29</v>
       </c>
       <c r="E42" s="15"/>
-      <c r="F42" s="41" t="s">
+      <c r="F42" s="42" t="s">
         <v>85</v>
       </c>
       <c r="G42">
@@ -6724,7 +6790,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="42"/>
+      <c r="A43" s="43"/>
       <c r="B43" s="9" t="s">
         <v>75</v>
       </c>
@@ -6735,7 +6801,7 @@
         <v>31</v>
       </c>
       <c r="E43" s="15"/>
-      <c r="F43" s="41"/>
+      <c r="F43" s="42"/>
       <c r="G43">
         <v>41</v>
       </c>
@@ -6744,7 +6810,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="42"/>
+      <c r="A44" s="43"/>
       <c r="B44" s="9" t="s">
         <v>75</v>
       </c>
@@ -6755,7 +6821,7 @@
         <v>32</v>
       </c>
       <c r="E44" s="15"/>
-      <c r="F44" s="41"/>
+      <c r="F44" s="42"/>
       <c r="G44">
         <v>42</v>
       </c>
@@ -6764,7 +6830,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="42"/>
+      <c r="A45" s="43"/>
       <c r="B45" s="9" t="s">
         <v>75</v>
       </c>
@@ -6775,7 +6841,7 @@
         <v>29</v>
       </c>
       <c r="E45" s="15"/>
-      <c r="F45" s="41"/>
+      <c r="F45" s="42"/>
       <c r="G45">
         <v>43</v>
       </c>
@@ -6784,7 +6850,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="42"/>
+      <c r="A46" s="43"/>
       <c r="B46" s="9" t="s">
         <v>75</v>
       </c>
@@ -6795,7 +6861,7 @@
         <v>31</v>
       </c>
       <c r="E46" s="15"/>
-      <c r="F46" s="41"/>
+      <c r="F46" s="42"/>
       <c r="G46">
         <v>44</v>
       </c>
@@ -6804,7 +6870,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="42"/>
+      <c r="A47" s="43"/>
       <c r="B47" s="9" t="s">
         <v>75</v>
       </c>
@@ -6815,7 +6881,7 @@
         <v>32</v>
       </c>
       <c r="E47" s="15"/>
-      <c r="F47" s="41"/>
+      <c r="F47" s="42"/>
       <c r="G47">
         <v>45</v>
       </c>
@@ -6824,7 +6890,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="37" t="s">
         <v>33</v>
       </c>
       <c r="B48" s="9" t="s">
@@ -6847,7 +6913,7 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A49" s="36"/>
+      <c r="A49" s="37"/>
       <c r="B49" s="9" t="s">
         <v>75</v>
       </c>
@@ -6869,7 +6935,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A50" s="36"/>
+      <c r="A50" s="37"/>
       <c r="B50" s="9" t="s">
         <v>75</v>
       </c>
@@ -6890,7 +6956,7 @@
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A51" s="36"/>
+      <c r="A51" s="37"/>
       <c r="B51" s="9" t="s">
         <v>75</v>
       </c>
@@ -6911,7 +6977,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A52" s="36" t="s">
+      <c r="A52" s="37" t="s">
         <v>62</v>
       </c>
       <c r="B52" s="9" t="s">
@@ -6934,7 +7000,7 @@
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A53" s="36"/>
+      <c r="A53" s="37"/>
       <c r="B53" s="9" t="s">
         <v>75</v>
       </c>
@@ -6963,7 +7029,7 @@
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A54" s="36"/>
+      <c r="A54" s="37"/>
       <c r="B54" s="9" t="s">
         <v>75</v>
       </c>
@@ -6992,7 +7058,7 @@
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A55" s="36"/>
+      <c r="A55" s="37"/>
       <c r="B55" s="9" t="s">
         <v>75</v>
       </c>
@@ -7034,7 +7100,7 @@
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A57" s="36" t="s">
+      <c r="A57" s="37" t="s">
         <v>137</v>
       </c>
       <c r="B57" s="9" t="s">
@@ -7058,7 +7124,7 @@
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A58" s="36"/>
+      <c r="A58" s="37"/>
       <c r="B58" s="9" t="s">
         <v>75</v>
       </c>
@@ -7080,7 +7146,7 @@
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A59" s="36"/>
+      <c r="A59" s="37"/>
       <c r="B59" s="9" t="s">
         <v>75</v>
       </c>
@@ -7102,7 +7168,7 @@
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A60" s="36"/>
+      <c r="A60" s="37"/>
       <c r="B60" s="9" t="s">
         <v>75</v>
       </c>
@@ -7124,7 +7190,7 @@
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A61" s="36" t="s">
+      <c r="A61" s="37" t="s">
         <v>138</v>
       </c>
       <c r="B61" s="9" t="s">
@@ -7148,7 +7214,7 @@
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A62" s="36"/>
+      <c r="A62" s="37"/>
       <c r="B62" s="9" t="s">
         <v>75</v>
       </c>
@@ -7170,7 +7236,7 @@
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A63" s="36"/>
+      <c r="A63" s="37"/>
       <c r="B63" s="9" t="s">
         <v>75</v>
       </c>
@@ -7192,7 +7258,7 @@
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A64" s="36"/>
+      <c r="A64" s="37"/>
       <c r="B64" s="9" t="s">
         <v>75</v>
       </c>
@@ -7214,7 +7280,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A65" s="36" t="s">
+      <c r="A65" s="37" t="s">
         <v>139</v>
       </c>
       <c r="B65" s="9" t="s">
@@ -7238,7 +7304,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A66" s="36"/>
+      <c r="A66" s="37"/>
       <c r="B66" s="9" t="s">
         <v>75</v>
       </c>
@@ -7260,7 +7326,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A67" s="36"/>
+      <c r="A67" s="37"/>
       <c r="B67" s="9" t="s">
         <v>75</v>
       </c>
@@ -7282,7 +7348,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" s="36"/>
+      <c r="A68" s="37"/>
       <c r="B68" s="9" t="s">
         <v>75</v>
       </c>
@@ -7304,7 +7370,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A69" s="36" t="s">
+      <c r="A69" s="37" t="s">
         <v>140</v>
       </c>
       <c r="B69" s="9" t="s">
@@ -7328,7 +7394,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A70" s="36"/>
+      <c r="A70" s="37"/>
       <c r="B70" s="9" t="s">
         <v>75</v>
       </c>
@@ -7350,7 +7416,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A71" s="36"/>
+      <c r="A71" s="37"/>
       <c r="B71" s="9" t="s">
         <v>75</v>
       </c>
@@ -7372,7 +7438,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A72" s="36"/>
+      <c r="A72" s="37"/>
       <c r="B72" s="9" t="s">
         <v>75</v>
       </c>
@@ -7691,7 +7757,7 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A87" s="36" t="s">
+      <c r="A87" s="37" t="s">
         <v>185</v>
       </c>
       <c r="B87" s="19" t="s">
@@ -7712,7 +7778,7 @@
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A88" s="36"/>
+      <c r="A88" s="37"/>
       <c r="B88" s="19" t="s">
         <v>76</v>
       </c>
@@ -7731,7 +7797,7 @@
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A89" s="36" t="s">
+      <c r="A89" s="37" t="s">
         <v>187</v>
       </c>
       <c r="B89" s="19" t="s">
@@ -7752,7 +7818,7 @@
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A90" s="36"/>
+      <c r="A90" s="37"/>
       <c r="B90" s="19" t="s">
         <v>76</v>
       </c>
@@ -7771,7 +7837,7 @@
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A91" s="36" t="s">
+      <c r="A91" s="37" t="s">
         <v>188</v>
       </c>
       <c r="B91" s="19" t="s">
@@ -7792,7 +7858,7 @@
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A92" s="36"/>
+      <c r="A92" s="37"/>
       <c r="B92" s="19" t="s">
         <v>76</v>
       </c>
@@ -7811,7 +7877,7 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A93" s="36"/>
+      <c r="A93" s="37"/>
       <c r="B93" s="19" t="s">
         <v>76</v>
       </c>
@@ -9918,6 +9984,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A91:A93"/>
+    <mergeCell ref="F42:F47"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="A89:A90"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A48:A51"/>
@@ -9926,12 +9998,6 @@
     <mergeCell ref="A61:A64"/>
     <mergeCell ref="A65:A68"/>
     <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A91:A93"/>
-    <mergeCell ref="F42:F47"/>
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="A89:A90"/>
   </mergeCells>
   <dataValidations count="21">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E19 E40" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">

</xml_diff>